<commit_message>
1. Improve map tooltip text 2. Changing greece bounding box so middle point is not on the sea
</commit_message>
<xml_diff>
--- a/epitweetr/inst/extdata/countries.xlsx
+++ b/epitweetr/inst/extdata/countries.xlsx
@@ -3279,8 +3279,8 @@
   </sheetPr>
   <dimension ref="A1:Q250"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q87" activeCellId="0" sqref="Q87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7454,16 +7454,16 @@
         <v>100</v>
       </c>
       <c r="N87" s="0" t="n">
-        <v>19.3098</v>
+        <v>19.25</v>
       </c>
       <c r="O87" s="0" t="n">
-        <v>34.5428</v>
+        <v>34.75</v>
       </c>
       <c r="P87" s="0" t="n">
-        <v>29.6527999</v>
+        <v>24.76</v>
       </c>
       <c r="Q87" s="0" t="n">
-        <v>41.7488784</v>
+        <v>41.73</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
1. Adding Default option "World (all)" and add option "World (geolocated)" 2. Change capitalisation of topics (e.g. Hepatitis A not Hepatitis a), with spelling/capitalisation as per topics list in this foler 3. Setting default alpha by topic on report and alerts based on excel file
</commit_message>
<xml_diff>
--- a/epitweetr/inst/extdata/countries.xlsx
+++ b/epitweetr/inst/extdata/countries.xlsx
@@ -3179,8 +3179,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -3247,12 +3248,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3277,10 +3282,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q250"/>
+  <dimension ref="A1:R250"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q87" activeCellId="0" sqref="Q87"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4038,6 +4047,7 @@
       <c r="Q16" s="0" t="n">
         <v>49.0390742051</v>
       </c>
+      <c r="R16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">

</xml_diff>

<commit_message>
1. Adding counts per selected location type and all types on line and map charts 2. Adding default timings to dashboard (7 days, 30 days, etc) 3. Adding kosovo as a country to making world geolocated match world all on map
</commit_message>
<xml_diff>
--- a/epitweetr/inst/extdata/countries.xlsx
+++ b/epitweetr/inst/extdata/countries.xlsx
@@ -11,7 +11,8 @@
     <sheet name="countries" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">countries!$A$1:$Q$250</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">countries!$A$1:$Q$251</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">countries!$A$1:$Q$250</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="1050">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1846" uniqueCount="1053">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -3173,6 +3174,15 @@
   </si>
   <si>
     <t xml:space="preserve">ISO 3166-2:ZW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kosovo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISO 3166-2:XK</t>
   </si>
 </sst>
 </file>
@@ -3181,7 +3191,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
+    <numFmt numFmtId="165" formatCode="&quot;BOOL&quot;E&quot;AN&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -3282,14 +3292,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R250"/>
+  <dimension ref="A1:R251"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="L261" activeCellId="0" sqref="L261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15162,8 +15172,50 @@
         <v>-15.6093188</v>
       </c>
     </row>
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="0" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B251" s="0" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D251" s="0" t="n">
+        <v>383</v>
+      </c>
+      <c r="E251" s="0" t="s">
+        <v>1052</v>
+      </c>
+      <c r="F251" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G251" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I251" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="J251" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="L251" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M251" s="1"/>
+      <c r="N251" s="0" t="n">
+        <v>19.7664</v>
+      </c>
+      <c r="O251" s="0" t="n">
+        <v>41.7713</v>
+      </c>
+      <c r="P251" s="0" t="n">
+        <v>21.9911</v>
+      </c>
+      <c r="Q251" s="0" t="n">
+        <v>43.2852</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Q250"/>
+  <autoFilter ref="A1:Q251"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>